<commit_message>
Update tests that did not pass
</commit_message>
<xml_diff>
--- a/src/test/resources/integration/Installed Software.xlsx
+++ b/src/test/resources/integration/Installed Software.xlsx
@@ -54,7 +54,7 @@
     <t>12.0.4518.1031</t>
   </si>
   <si>
-    <t>Microsoft_1663504721301</t>
+    <t>Microsoft_1663510154692</t>
   </si>
   <si>
     <t>IntTest BadApps-Bad-Apps</t>
@@ -69,7 +69,7 @@
     <t>4.9.01095</t>
   </si>
   <si>
-    <t>CISCO_1663504721459</t>
+    <t>CISCO_1663510154750</t>
   </si>
   <si>
     <t>FortiClient</t>
@@ -81,7 +81,7 @@
     <t>6.0.7.0243</t>
   </si>
   <si>
-    <t>Fortinet_1663504721542</t>
+    <t>Fortinet_1663510154817</t>
   </si>
   <si>
     <t>Citrix Workspace(DV)</t>
@@ -93,7 +93,7 @@
     <t>20.11.0.26</t>
   </si>
   <si>
-    <t>Citrix_1663504721650</t>
+    <t>Citrix_1663510154851</t>
   </si>
   <si>
     <t>Citrix Authentication Manager</t>
@@ -105,7 +105,7 @@
     <t>20.11.0.12</t>
   </si>
   <si>
-    <t>Citrix_1663504721710</t>
+    <t>Citrix_1663510154901</t>
   </si>
   <si>
     <t>{8CA6F29E-DF02-4519-B33C-9AC9935D28E9}</t>
@@ -114,7 +114,7 @@
     <t>20.11.0.13</t>
   </si>
   <si>
-    <t>Citrix_1663504721766</t>
+    <t>Citrix_1663510154935</t>
   </si>
   <si>
     <t>Microsoft Visual C++ 2019 X86 Minimum Runtime - 14.24.28127</t>
@@ -126,7 +126,7 @@
     <t>14.24.28127</t>
   </si>
   <si>
-    <t>Microsoft_1663504721822</t>
+    <t>Microsoft_1663510154970</t>
   </si>
   <si>
     <t>Java Auto Updater</t>
@@ -138,7 +138,7 @@
     <t>2.8.231.11</t>
   </si>
   <si>
-    <t>Oracle_1663504721909</t>
+    <t>Oracle_1663510155011</t>
   </si>
   <si>
     <t>PHP Manager 1.4 for IIS 10</t>
@@ -150,7 +150,7 @@
     <t>1.4.0</t>
   </si>
   <si>
-    <t>Vendor_1663504722012</t>
+    <t>Vendor_1663510155044</t>
   </si>
   <si>
     <t>Test App duplicate ID</t>
@@ -159,7 +159,7 @@
     <t>1.0.2.2</t>
   </si>
   <si>
-    <t>Test_1663504722068</t>
+    <t>Test_1663510155080</t>
   </si>
   <si>
     <t>Test App 2</t>
@@ -171,7 +171,7 @@
     <t>9.4.5</t>
   </si>
   <si>
-    <t>Test_1663504722155</t>
+    <t>Test_1663510155127</t>
   </si>
   <si>
     <t>IntTest BadApps-Bad-AppsIntTest GoodApps-DESKTOP-1GTK0TB;</t>
@@ -186,7 +186,7 @@
     <t>2.6.8627.1</t>
   </si>
   <si>
-    <t>Waves_1663504722365</t>
+    <t>Waves_1663510155264</t>
   </si>
   <si>
     <t>IntTest GoodApps-DESKTOP-1GTK0TB</t>
@@ -201,7 +201,7 @@
     <t>20.12.0.10</t>
   </si>
   <si>
-    <t>Citrix_1663504722410</t>
+    <t>Citrix_1663510155312</t>
   </si>
   <si>
     <t>Microsoft Web Platform Installer 5.1</t>
@@ -213,7 +213,7 @@
     <t>5.1.51515.0</t>
   </si>
   <si>
-    <t>Microsoft_1663504722470</t>
+    <t>Microsoft_1663510155345</t>
   </si>
   <si>
     <t>Java 8 Update 231</t>
@@ -225,7 +225,7 @@
     <t>8.0.2310.11</t>
   </si>
   <si>
-    <t>Oracle_1663504722522</t>
+    <t>Oracle_1663510155384</t>
   </si>
   <si>
     <t>Check Point SSL Network Extender Service</t>
@@ -237,7 +237,7 @@
     <t>7.01.0000</t>
   </si>
   <si>
-    <t>CheckPoint_1663504722565</t>
+    <t>CheckPoint_1663510155424</t>
   </si>
   <si>
     <t>Adobe Acrobat Reader DC</t>
@@ -249,7 +249,7 @@
     <t>22.002.20191</t>
   </si>
   <si>
-    <t>Adobe_1663504722621</t>
+    <t>Adobe_1663510155457</t>
   </si>
   <si>
     <t>Citrix Screen Casting for Windows</t>
@@ -261,7 +261,7 @@
     <t>19.11.100.48</t>
   </si>
   <si>
-    <t>Citrix_1663504722667</t>
+    <t>Citrix_1663510155486</t>
   </si>
   <si>
     <t>Check Point VPN</t>
@@ -273,7 +273,7 @@
     <t>98.61.1703</t>
   </si>
   <si>
-    <t>CheckPoint_1663504722725</t>
+    <t>CheckPoint_1663510155521</t>
   </si>
   <si>
     <t>Crystal Reports XI Release 2</t>
@@ -285,7 +285,7 @@
     <t>11.5.0.31327</t>
   </si>
   <si>
-    <t>Business_1663504722758</t>
+    <t>Business_1663510155555</t>
   </si>
   <si>
     <t>ConnectWise Manage Client 64-bit</t>
@@ -297,7 +297,7 @@
     <t>20.3.1</t>
   </si>
   <si>
-    <t>ConnectWise_1663504722795</t>
+    <t>ConnectWise_1663510155589</t>
   </si>
   <si>
     <t>Cisco Webex Meetings</t>
@@ -309,7 +309,7 @@
     <t>39.9.2.116</t>
   </si>
   <si>
-    <t>CISCO_1663504722836</t>
+    <t>CISCO_1663510155618</t>
   </si>
   <si>
     <t>SAP Crystal Reports runtime engine for .NET Framework (64-bit)</t>
@@ -321,7 +321,7 @@
     <t>13.0.15.1840</t>
   </si>
   <si>
-    <t>SAP_1663504722874</t>
+    <t>SAP_1663510155645</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Revert to last commit and create branch for Vendor Accronym
</commit_message>
<xml_diff>
--- a/src/test/resources/integration/Installed Software.xlsx
+++ b/src/test/resources/integration/Installed Software.xlsx
@@ -54,7 +54,7 @@
     <t>12.0.4518.1031</t>
   </si>
   <si>
-    <t>Microsoft_1663510154692</t>
+    <t>Microsoft_1663605558641</t>
   </si>
   <si>
     <t>IntTest BadApps-Bad-Apps</t>
@@ -69,7 +69,7 @@
     <t>4.9.01095</t>
   </si>
   <si>
-    <t>CISCO_1663510154750</t>
+    <t>CISCO_1663605558782</t>
   </si>
   <si>
     <t>FortiClient</t>
@@ -81,7 +81,7 @@
     <t>6.0.7.0243</t>
   </si>
   <si>
-    <t>Fortinet_1663510154817</t>
+    <t>Fortinet_1663605558910</t>
   </si>
   <si>
     <t>Citrix Workspace(DV)</t>
@@ -93,7 +93,7 @@
     <t>20.11.0.26</t>
   </si>
   <si>
-    <t>Citrix_1663510154851</t>
+    <t>Citrix_1663605558995</t>
   </si>
   <si>
     <t>Citrix Authentication Manager</t>
@@ -105,7 +105,7 @@
     <t>20.11.0.12</t>
   </si>
   <si>
-    <t>Citrix_1663510154901</t>
+    <t>Citrix_1663605559148</t>
   </si>
   <si>
     <t>{8CA6F29E-DF02-4519-B33C-9AC9935D28E9}</t>
@@ -114,7 +114,7 @@
     <t>20.11.0.13</t>
   </si>
   <si>
-    <t>Citrix_1663510154935</t>
+    <t>Citrix_1663605559236</t>
   </si>
   <si>
     <t>Microsoft Visual C++ 2019 X86 Minimum Runtime - 14.24.28127</t>
@@ -126,7 +126,7 @@
     <t>14.24.28127</t>
   </si>
   <si>
-    <t>Microsoft_1663510154970</t>
+    <t>Microsoft_1663605559303</t>
   </si>
   <si>
     <t>Java Auto Updater</t>
@@ -138,7 +138,7 @@
     <t>2.8.231.11</t>
   </si>
   <si>
-    <t>Oracle_1663510155011</t>
+    <t>Oracle_1663605559389</t>
   </si>
   <si>
     <t>PHP Manager 1.4 for IIS 10</t>
@@ -150,7 +150,7 @@
     <t>1.4.0</t>
   </si>
   <si>
-    <t>Vendor_1663510155044</t>
+    <t>Vendor_1663605559563</t>
   </si>
   <si>
     <t>Test App duplicate ID</t>
@@ -159,7 +159,7 @@
     <t>1.0.2.2</t>
   </si>
   <si>
-    <t>Test_1663510155080</t>
+    <t>Test_1663605559611</t>
   </si>
   <si>
     <t>Test App 2</t>
@@ -171,7 +171,7 @@
     <t>9.4.5</t>
   </si>
   <si>
-    <t>Test_1663510155127</t>
+    <t>Test_1663605559732</t>
   </si>
   <si>
     <t>IntTest BadApps-Bad-AppsIntTest GoodApps-DESKTOP-1GTK0TB;</t>
@@ -186,7 +186,7 @@
     <t>2.6.8627.1</t>
   </si>
   <si>
-    <t>Waves_1663510155264</t>
+    <t>Waves_1663605559984</t>
   </si>
   <si>
     <t>IntTest GoodApps-DESKTOP-1GTK0TB</t>
@@ -201,7 +201,7 @@
     <t>20.12.0.10</t>
   </si>
   <si>
-    <t>Citrix_1663510155312</t>
+    <t>Citrix_1663605560032</t>
   </si>
   <si>
     <t>Microsoft Web Platform Installer 5.1</t>
@@ -213,7 +213,7 @@
     <t>5.1.51515.0</t>
   </si>
   <si>
-    <t>Microsoft_1663510155345</t>
+    <t>Microsoft_1663605560077</t>
   </si>
   <si>
     <t>Java 8 Update 231</t>
@@ -225,7 +225,7 @@
     <t>8.0.2310.11</t>
   </si>
   <si>
-    <t>Oracle_1663510155384</t>
+    <t>Oracle_1663605560197</t>
   </si>
   <si>
     <t>Check Point SSL Network Extender Service</t>
@@ -237,7 +237,7 @@
     <t>7.01.0000</t>
   </si>
   <si>
-    <t>CheckPoint_1663510155424</t>
+    <t>CheckPoint_1663605560240</t>
   </si>
   <si>
     <t>Adobe Acrobat Reader DC</t>
@@ -249,7 +249,7 @@
     <t>22.002.20191</t>
   </si>
   <si>
-    <t>Adobe_1663510155457</t>
+    <t>Adobe_1663605560295</t>
   </si>
   <si>
     <t>Citrix Screen Casting for Windows</t>
@@ -261,7 +261,7 @@
     <t>19.11.100.48</t>
   </si>
   <si>
-    <t>Citrix_1663510155486</t>
+    <t>Citrix_1663605560333</t>
   </si>
   <si>
     <t>Check Point VPN</t>
@@ -273,7 +273,7 @@
     <t>98.61.1703</t>
   </si>
   <si>
-    <t>CheckPoint_1663510155521</t>
+    <t>CheckPoint_1663605560437</t>
   </si>
   <si>
     <t>Crystal Reports XI Release 2</t>
@@ -285,7 +285,7 @@
     <t>11.5.0.31327</t>
   </si>
   <si>
-    <t>Business_1663510155555</t>
+    <t>Business_1663605560472</t>
   </si>
   <si>
     <t>ConnectWise Manage Client 64-bit</t>
@@ -297,7 +297,7 @@
     <t>20.3.1</t>
   </si>
   <si>
-    <t>ConnectWise_1663510155589</t>
+    <t>ConnectWise_1663605560672</t>
   </si>
   <si>
     <t>Cisco Webex Meetings</t>
@@ -309,7 +309,7 @@
     <t>39.9.2.116</t>
   </si>
   <si>
-    <t>CISCO_1663510155618</t>
+    <t>CISCO_1663605560710</t>
   </si>
   <si>
     <t>SAP Crystal Reports runtime engine for .NET Framework (64-bit)</t>
@@ -321,7 +321,7 @@
     <t>13.0.15.1840</t>
   </si>
   <si>
-    <t>SAP_1663510155645</t>
+    <t>SAP_1663605560866</t>
   </si>
 </sst>
 </file>

</xml_diff>